<commit_message>
Ajuste nuevas ligas, porteros y métricas
</commit_message>
<xml_diff>
--- a/ponderacion_competencias.xlsx
+++ b/ponderacion_competencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelDuran\AppData\Local\Programs\Python\streamlit_scouting_gk\streamlit_scouting_gk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D8505A-FB13-4DA9-800C-12B2CEBBD4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097DC12F-77AE-4E6F-9351-C549B988A96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Competencia</t>
   </si>
@@ -113,6 +113,42 @@
   </si>
   <si>
     <t>Turkey Super Lig</t>
+  </si>
+  <si>
+    <t>Belgian Challenger Pro League</t>
+  </si>
+  <si>
+    <t>Chile Primera</t>
+  </si>
+  <si>
+    <t>Colombia Superliga</t>
+  </si>
+  <si>
+    <t>CONMEBOL Libertadores U20</t>
+  </si>
+  <si>
+    <t>CONMEBOL U17</t>
+  </si>
+  <si>
+    <t>CONMEBOL U20</t>
+  </si>
+  <si>
+    <t>Dutch Eerste Divisie</t>
+  </si>
+  <si>
+    <t>Ecuador Liga Pro</t>
+  </si>
+  <si>
+    <t>French Ligue 2</t>
+  </si>
+  <si>
+    <t>UEFA Under 17 Championship</t>
+  </si>
+  <si>
+    <t>UEFA Under 19 Championship</t>
+  </si>
+  <si>
+    <t>UEFA Under 21 Championship</t>
   </si>
 </sst>
 </file>
@@ -475,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -513,7 +549,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1.9</v>
@@ -521,7 +557,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1.9</v>
@@ -529,7 +565,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>1.9</v>
@@ -553,23 +589,23 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>1.3</v>
@@ -577,7 +613,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>1.2</v>
@@ -585,7 +621,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>1.2</v>
@@ -593,7 +629,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1.1000000000000001</v>
@@ -601,7 +637,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>1.1000000000000001</v>
@@ -633,7 +669,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -641,7 +677,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -649,7 +685,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -665,63 +701,159 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B23">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B24">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B25">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B26">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B28">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B41">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B29">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B41">
       <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
sin ponderacion por ligas
</commit_message>
<xml_diff>
--- a/ponderacion_competencias.xlsx
+++ b/ponderacion_competencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelDuran\AppData\Local\Programs\Python\streamlit_scouting_gk\streamlit_scouting_gk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097DC12F-77AE-4E6F-9351-C549B988A96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F8F971-9A03-40B8-8E21-C15BAE883F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -536,7 +536,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>1.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>1.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -552,7 +552,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>1.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -560,7 +560,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>1.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -568,7 +568,7 @@
         <v>26</v>
       </c>
       <c r="B6">
-        <v>1.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -576,7 +576,7 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>1.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -584,7 +584,7 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -592,7 +592,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>1.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -600,7 +600,7 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>1.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -608,7 +608,7 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>1.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -616,7 +616,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -624,7 +624,7 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -632,7 +632,7 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -640,7 +640,7 @@
         <v>27</v>
       </c>
       <c r="B15">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -728,7 +728,7 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
@@ -736,7 +736,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
@@ -768,7 +768,7 @@
         <v>37</v>
       </c>
       <c r="B31">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
@@ -776,7 +776,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -784,7 +784,7 @@
         <v>30</v>
       </c>
       <c r="B33">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -792,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="B34">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -800,7 +800,7 @@
         <v>36</v>
       </c>
       <c r="B35">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
@@ -808,7 +808,7 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
@@ -816,7 +816,7 @@
         <v>21</v>
       </c>
       <c r="B37">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -824,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="B38">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -832,7 +832,7 @@
         <v>23</v>
       </c>
       <c r="B39">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
@@ -840,7 +840,7 @@
         <v>25</v>
       </c>
       <c r="B40">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
@@ -848,7 +848,7 @@
         <v>28</v>
       </c>
       <c r="B41">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>